<commit_message>
feat: versiona cambios pendientes de taller, servicios externos y tipo de cambio
Se versionan cambios de backend y frontend para módulo de taller:
- Integración de servicios externos (controladores, modelos, rutas y modales)
- Ajustes de tipo de cambio (FxRate/FxRateType, rutas, servicios y vistas)
- Soporte de imágenes para metales/cliente en flujo de taller
- Actualizaciones en ventas/usuarios y configuración asociada
- Scripts de apoyo y migraciones SQL relacionadas
- Documentación y archivos operativos actualizados
</commit_message>
<xml_diff>
--- a/Documents/Actividades realizadas/ActividadesN__.xlsx
+++ b/Documents/Actividades realizadas/ActividadesN__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\1.- VioletaSystem\Documents\Actividades realizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FD7B7D-1A0A-44A7-8392-AD4F8BF9BD01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09807BA6-07F8-447D-B203-C2D889F5EE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="331">
   <si>
     <t>Descripción</t>
   </si>
@@ -982,6 +982,54 @@
   </si>
   <si>
     <t>Estructura de SQL de Metal Agranel, así como su alta, modificación, eliminación y consulta de lista</t>
+  </si>
+  <si>
+    <t>Carga y descarga de imágenes en los activos del cliente, manejo de carrusel para la mejor visualización</t>
+  </si>
+  <si>
+    <t>Estructura de SQL de Activo del cliente, así como su alta, modificación, eliminación y consulta de lista</t>
+  </si>
+  <si>
+    <t>Reunion con Martín para ver los avances de los sobres y tomar sus nuevas indicaciones</t>
+  </si>
+  <si>
+    <t>Calculo de monto del metal por kilataje en la sección metal agranel</t>
+  </si>
+  <si>
+    <t>Manejo completo de los servicios externos, alta, modificación, eliminación y consulta</t>
+  </si>
+  <si>
+    <t>Alimentación de la mano de obra, alta, modificación, eliminación y consulta de la sección de mano de obra</t>
+  </si>
+  <si>
+    <t>Navegación entre los campos en toda la pantalla de taller</t>
+  </si>
+  <si>
+    <t>Manejo de Imágenes para el encabezado de taller, asi como en el metal del cliente</t>
+  </si>
+  <si>
+    <t>Butones para pasar de ventas a taller y biseversa</t>
+  </si>
+  <si>
+    <t>Agregar el destajo en los usuarios</t>
+  </si>
+  <si>
+    <t>Agregar el total de taller en la parte superior</t>
+  </si>
+  <si>
+    <t>Cambio de producto por definir por un producto ya registrado</t>
+  </si>
+  <si>
+    <t>Se agregan botones para cambiar Estatus el taller  de cotización a Pedido de taller, asignado, Finalizado/Mostrador, Entregado</t>
+  </si>
+  <si>
+    <t>Agregar pagos en nuevos taller</t>
+  </si>
+  <si>
+    <t>Actualización de pantalla para el manejo de tipos de cambio en Oro, Dólar, Plata diferentes Kilatajes, etc, asi como la alimentación, edición, actualziación y eliminación de nuevas referencias para los tipos de cambios</t>
+  </si>
+  <si>
+    <t>Reunión mostrando el avance de taller</t>
   </si>
 </sst>
 </file>
@@ -1436,30 +1484,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="3" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1475,6 +1499,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1483,6 +1510,27 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="10" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1818,11 +1866,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K350"/>
+  <dimension ref="A1:K364"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A298" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F306" sqref="F306"/>
+      <pane ySplit="1" topLeftCell="A314" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C322" sqref="C322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7627,7 +7675,7 @@
       <c r="F296" s="2">
         <v>0.76041666666666663</v>
       </c>
-      <c r="H296" s="14">
+      <c r="H296" s="20">
         <v>2</v>
       </c>
     </row>
@@ -7645,7 +7693,7 @@
       <c r="F297" s="2">
         <v>0.55208333333333337</v>
       </c>
-      <c r="H297" s="14">
+      <c r="H297" s="20">
         <v>1</v>
       </c>
     </row>
@@ -7663,7 +7711,7 @@
       <c r="F298" s="2">
         <v>0.70138888888888884</v>
       </c>
-      <c r="H298" s="14">
+      <c r="H298" s="20">
         <v>1</v>
       </c>
     </row>
@@ -7681,7 +7729,7 @@
       <c r="F299" s="2">
         <v>0.88263888888888886</v>
       </c>
-      <c r="H299" s="14">
+      <c r="H299" s="20">
         <v>1.5</v>
       </c>
     </row>
@@ -7699,7 +7747,7 @@
       <c r="F300" s="2">
         <v>0.93611111111111112</v>
       </c>
-      <c r="H300" s="14">
+      <c r="H300" s="20">
         <v>1</v>
       </c>
     </row>
@@ -7717,13 +7765,13 @@
       <c r="F301" s="2">
         <v>0.47222222222222221</v>
       </c>
-      <c r="H301" s="14">
+      <c r="H301" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="302" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A302" s="5"/>
-      <c r="C302" s="61">
+      <c r="C302" s="9">
         <v>46062</v>
       </c>
       <c r="D302" s="13" t="s">
@@ -7735,13 +7783,13 @@
       <c r="F302" s="2">
         <v>0.67361111111111116</v>
       </c>
-      <c r="H302" s="14">
+      <c r="H302" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A303" s="5"/>
-      <c r="C303" s="61">
+      <c r="C303" s="9">
         <v>46063</v>
       </c>
       <c r="D303" s="13" t="s">
@@ -7753,13 +7801,13 @@
       <c r="F303" s="2">
         <v>0.52430555555555558</v>
       </c>
-      <c r="H303" s="14">
+      <c r="H303" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="304" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A304" s="5"/>
-      <c r="C304" s="61">
+      <c r="C304" s="9">
         <v>46063</v>
       </c>
       <c r="D304" s="13" t="s">
@@ -7771,13 +7819,13 @@
       <c r="F304" s="2">
         <v>0.71527777777777779</v>
       </c>
-      <c r="H304" s="14">
+      <c r="H304" s="20">
         <v>4</v>
       </c>
     </row>
-    <row r="305" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A305" s="5"/>
-      <c r="C305" s="61">
+      <c r="C305" s="9">
         <v>46063</v>
       </c>
       <c r="D305" s="13" t="s">
@@ -7789,343 +7837,497 @@
       <c r="F305" s="2">
         <v>0.84375</v>
       </c>
-      <c r="H305" s="14">
+      <c r="H305" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A306" s="5"/>
-      <c r="C306" s="61"/>
-      <c r="D306" s="13"/>
+      <c r="C306" s="9"/>
+      <c r="D306" s="13" t="s">
+        <v>316</v>
+      </c>
       <c r="E306" s="2"/>
       <c r="F306" s="2"/>
-    </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H306" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="307" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A307" s="5"/>
-      <c r="C307" s="61"/>
-      <c r="D307" s="13"/>
-      <c r="E307" s="2"/>
-      <c r="F307" s="2"/>
-    </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C307" s="9">
+        <v>46063</v>
+      </c>
+      <c r="D307" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="E307" s="2">
+        <v>0.84375</v>
+      </c>
+      <c r="F307" s="2">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="H307" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="308" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A308" s="5"/>
-      <c r="C308" s="61"/>
-      <c r="D308" s="13"/>
-      <c r="E308" s="2"/>
-      <c r="F308" s="2"/>
-    </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C308" s="9">
+        <v>46064</v>
+      </c>
+      <c r="D308" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="E308" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="F308" s="2">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="H308" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A309" s="5"/>
-      <c r="C309" s="61"/>
-      <c r="D309" s="13"/>
-      <c r="E309" s="2"/>
-      <c r="F309" s="2"/>
-    </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C309" s="9">
+        <v>46073</v>
+      </c>
+      <c r="D309" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="E309" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F309" s="2">
+        <v>0.63888888888888884</v>
+      </c>
+      <c r="H309" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="310" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A310" s="5"/>
-      <c r="E310" s="2"/>
-      <c r="F310" s="2"/>
-    </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A311" s="74" t="s">
+      <c r="C310" s="9"/>
+      <c r="D310" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="E310" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F310" s="2">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="H310" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A311" s="5"/>
+      <c r="C311" s="9">
+        <v>46074</v>
+      </c>
+      <c r="D311" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="E311" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="F311" s="2">
+        <v>0.46527777777777779</v>
+      </c>
+      <c r="H311" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A312" s="5"/>
+      <c r="C312" s="9">
+        <v>46074</v>
+      </c>
+      <c r="D312" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="E312" s="2">
+        <v>0.47222222222222221</v>
+      </c>
+      <c r="F312" s="2">
+        <v>0.55694444444444446</v>
+      </c>
+      <c r="H312" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="313" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A313" s="5"/>
+      <c r="C313" s="9">
+        <v>46074</v>
+      </c>
+      <c r="D313" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="E313" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F313" s="2">
+        <v>0.71875</v>
+      </c>
+      <c r="H313" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="314" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A314" s="5"/>
+      <c r="C314" s="9">
+        <v>46074</v>
+      </c>
+      <c r="D314" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="E314" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="F314" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H314" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A315" s="5"/>
+      <c r="C315" s="9">
+        <v>46074</v>
+      </c>
+      <c r="D315" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="E315" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F315" s="2">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="H315" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A316" s="5"/>
+      <c r="C316" s="9">
+        <v>46074</v>
+      </c>
+      <c r="D316" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="E316" s="2">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="F316" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="H316" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A317" s="5"/>
+      <c r="C317" s="9">
+        <v>46074</v>
+      </c>
+      <c r="D317" s="13" t="s">
+        <v>325</v>
+      </c>
+      <c r="E317" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="F317" s="2">
+        <v>0.8979166666666667</v>
+      </c>
+      <c r="H317" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A318" s="5"/>
+      <c r="C318" s="9">
+        <v>46076</v>
+      </c>
+      <c r="D318" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="E318" s="2">
+        <v>0.8979166666666667</v>
+      </c>
+      <c r="F318" s="2">
+        <v>0.9555555555555556</v>
+      </c>
+      <c r="H318" s="14">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="319" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A319" s="5"/>
+      <c r="C319" s="9">
+        <v>46076</v>
+      </c>
+      <c r="D319" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="E319" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="F319" s="2">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="H319" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A320" s="5"/>
+      <c r="C320" s="9">
+        <v>46076</v>
+      </c>
+      <c r="D320" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="E320" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F320" s="2">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="H320" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A321" s="5"/>
+      <c r="C321" s="61">
+        <v>46078</v>
+      </c>
+      <c r="D321" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="E321" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F321" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="H321" s="14">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A322" s="5"/>
+      <c r="C322" s="61"/>
+      <c r="D322" s="13"/>
+      <c r="E322" s="2"/>
+      <c r="F322" s="2"/>
+    </row>
+    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A323" s="5"/>
+      <c r="C323" s="61"/>
+      <c r="D323" s="13"/>
+      <c r="E323" s="2"/>
+      <c r="F323" s="2"/>
+    </row>
+    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A324" s="5"/>
+      <c r="E324" s="2"/>
+      <c r="F324" s="2"/>
+    </row>
+    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A325" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="B311" s="74"/>
-      <c r="C311" s="74"/>
-      <c r="D311" s="74"/>
-      <c r="E311" s="74"/>
-      <c r="F311" s="74"/>
-      <c r="G311" s="16">
-        <f>SUM(G2:G310)</f>
+      <c r="B325" s="83"/>
+      <c r="C325" s="83"/>
+      <c r="D325" s="83"/>
+      <c r="E325" s="83"/>
+      <c r="F325" s="83"/>
+      <c r="G325" s="16">
+        <f>SUM(G2:G324)</f>
         <v>314.78999999999996</v>
       </c>
-      <c r="H311" s="16">
-        <f>SUM(H2:H310)</f>
-        <v>127.8</v>
-      </c>
-    </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A312" s="74" t="s">
+      <c r="H325" s="16">
+        <f>SUM(H2:H324)</f>
+        <v>160.30000000000001</v>
+      </c>
+    </row>
+    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A326" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="B312" s="74"/>
-      <c r="C312" s="74"/>
-      <c r="D312" s="74"/>
-      <c r="E312" s="74"/>
-      <c r="F312" s="74"/>
-      <c r="G312" s="16">
+      <c r="B326" s="83"/>
+      <c r="C326" s="83"/>
+      <c r="D326" s="83"/>
+      <c r="E326" s="83"/>
+      <c r="F326" s="83"/>
+      <c r="G326" s="16">
         <v>200</v>
       </c>
-      <c r="H312" s="16">
+      <c r="H326" s="16">
         <v>300</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A313" s="74" t="s">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A327" s="83" t="s">
         <v>84</v>
       </c>
-      <c r="B313" s="74"/>
-      <c r="C313" s="74"/>
-      <c r="D313" s="74"/>
-      <c r="E313" s="74"/>
-      <c r="F313" s="74"/>
-      <c r="G313" s="17">
-        <f>G312*G311</f>
+      <c r="B327" s="83"/>
+      <c r="C327" s="83"/>
+      <c r="D327" s="83"/>
+      <c r="E327" s="83"/>
+      <c r="F327" s="83"/>
+      <c r="G327" s="17">
+        <f>G326*G325</f>
         <v>62957.999999999993</v>
       </c>
-      <c r="H313" s="18">
-        <f>H312*H311</f>
-        <v>38340</v>
-      </c>
-      <c r="J313">
+      <c r="H327" s="18">
+        <f>H326*H325</f>
+        <v>48090</v>
+      </c>
+      <c r="J327">
         <v>-500</v>
       </c>
     </row>
-    <row r="314" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A314" s="74" t="s">
+    <row r="328" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A328" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="B314" s="74"/>
-      <c r="C314" s="74"/>
-      <c r="D314" s="74"/>
-      <c r="E314" s="74"/>
-      <c r="F314" s="74"/>
-      <c r="G314" s="79">
-        <f>G313+H313</f>
-        <v>101298</v>
-      </c>
-      <c r="H314" s="79"/>
-    </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A315" s="10"/>
-      <c r="B315" s="82" t="s">
+      <c r="B328" s="83"/>
+      <c r="C328" s="83"/>
+      <c r="D328" s="83"/>
+      <c r="E328" s="83"/>
+      <c r="F328" s="83"/>
+      <c r="G328" s="71">
+        <f>G327+H327</f>
+        <v>111048</v>
+      </c>
+      <c r="H328" s="71"/>
+    </row>
+    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A329" s="10"/>
+      <c r="B329" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="C315" s="82"/>
-      <c r="D315" s="82"/>
-      <c r="E315" s="82"/>
-      <c r="F315" s="82"/>
-      <c r="G315" s="21"/>
-    </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A316" s="11">
+      <c r="C329" s="74"/>
+      <c r="D329" s="74"/>
+      <c r="E329" s="74"/>
+      <c r="F329" s="74"/>
+      <c r="G329" s="21"/>
+    </row>
+    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A330" s="11">
         <v>45109</v>
       </c>
-      <c r="B316" s="83" t="s">
+      <c r="B330" s="75" t="s">
         <v>59</v>
       </c>
-      <c r="C316" s="83"/>
-      <c r="D316" s="83"/>
-      <c r="E316" s="83"/>
-      <c r="F316" s="83"/>
-      <c r="G316" s="84">
+      <c r="C330" s="75"/>
+      <c r="D330" s="75"/>
+      <c r="E330" s="75"/>
+      <c r="F330" s="75"/>
+      <c r="G330" s="77">
         <v>10000</v>
       </c>
-      <c r="H316" s="84"/>
-    </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A317" s="11"/>
-      <c r="B317" s="86" t="s">
+      <c r="H330" s="77"/>
+    </row>
+    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A331" s="11"/>
+      <c r="B331" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="C317" s="86"/>
-      <c r="D317" s="86"/>
-      <c r="E317" s="86"/>
-      <c r="F317" s="86"/>
-      <c r="G317" s="84">
+      <c r="C331" s="79"/>
+      <c r="D331" s="79"/>
+      <c r="E331" s="79"/>
+      <c r="F331" s="79"/>
+      <c r="G331" s="77">
         <v>5000</v>
       </c>
-      <c r="H317" s="84"/>
-    </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A318" s="11">
+      <c r="H331" s="77"/>
+    </row>
+    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A332" s="11">
         <v>45278</v>
       </c>
-      <c r="B318" s="75" t="s">
+      <c r="B332" s="76" t="s">
         <v>96</v>
       </c>
-      <c r="C318" s="75"/>
-      <c r="D318" s="75"/>
-      <c r="E318" s="75"/>
-      <c r="F318" s="75"/>
-      <c r="G318" s="84">
+      <c r="C332" s="76"/>
+      <c r="D332" s="76"/>
+      <c r="E332" s="76"/>
+      <c r="F332" s="76"/>
+      <c r="G332" s="77">
         <v>9800</v>
       </c>
-      <c r="H318" s="84"/>
-    </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A319" s="11"/>
-      <c r="B319" s="75"/>
-      <c r="C319" s="75"/>
-      <c r="D319" s="75"/>
-      <c r="E319" s="75"/>
-      <c r="F319" s="75"/>
-      <c r="G319" s="85"/>
-      <c r="H319" s="85"/>
-    </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A320" s="11"/>
-      <c r="B320" s="75"/>
-      <c r="C320" s="75"/>
-      <c r="D320" s="75"/>
-      <c r="E320" s="75"/>
-      <c r="F320" s="75"/>
-      <c r="G320" s="85"/>
-      <c r="H320" s="85"/>
-    </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A321" s="11"/>
-      <c r="B321" s="75"/>
-      <c r="C321" s="75"/>
-      <c r="D321" s="75"/>
-      <c r="E321" s="75"/>
-      <c r="F321" s="75"/>
-      <c r="G321" s="85"/>
-      <c r="H321" s="85"/>
-    </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A322" s="11"/>
-      <c r="B322" s="75" t="s">
+      <c r="H332" s="77"/>
+    </row>
+    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A333" s="11"/>
+      <c r="B333" s="76"/>
+      <c r="C333" s="76"/>
+      <c r="D333" s="76"/>
+      <c r="E333" s="76"/>
+      <c r="F333" s="76"/>
+      <c r="G333" s="78"/>
+      <c r="H333" s="78"/>
+    </row>
+    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A334" s="11"/>
+      <c r="B334" s="76"/>
+      <c r="C334" s="76"/>
+      <c r="D334" s="76"/>
+      <c r="E334" s="76"/>
+      <c r="F334" s="76"/>
+      <c r="G334" s="78"/>
+      <c r="H334" s="78"/>
+    </row>
+    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A335" s="11"/>
+      <c r="B335" s="76"/>
+      <c r="C335" s="76"/>
+      <c r="D335" s="76"/>
+      <c r="E335" s="76"/>
+      <c r="F335" s="76"/>
+      <c r="G335" s="78"/>
+      <c r="H335" s="78"/>
+    </row>
+    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A336" s="11"/>
+      <c r="B336" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="C322" s="75"/>
-      <c r="D322" s="75"/>
-      <c r="E322" s="75"/>
-      <c r="F322" s="75"/>
-      <c r="G322" s="84">
-        <f>SUM(G316:H321)</f>
+      <c r="C336" s="76"/>
+      <c r="D336" s="76"/>
+      <c r="E336" s="76"/>
+      <c r="F336" s="76"/>
+      <c r="G336" s="77">
+        <f>SUM(G330:H335)</f>
         <v>24800</v>
       </c>
-      <c r="H322" s="84"/>
-    </row>
-    <row r="323" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A323" s="80" t="s">
+      <c r="H336" s="77"/>
+    </row>
+    <row r="337" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A337" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="B323" s="80"/>
-      <c r="C323" s="80"/>
-      <c r="D323" s="80"/>
-      <c r="E323" s="80"/>
-      <c r="F323" s="80"/>
-      <c r="G323" s="81">
-        <f>G314-G322</f>
-        <v>76498</v>
-      </c>
-      <c r="H323" s="81"/>
-    </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A324" s="11"/>
-      <c r="B324" s="12"/>
-      <c r="C324" s="12"/>
-      <c r="D324" s="12"/>
-      <c r="E324" s="12"/>
-      <c r="F324" s="12"/>
-    </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A325" s="11"/>
-      <c r="B325" s="12"/>
-      <c r="C325" s="12"/>
-      <c r="D325" s="12"/>
-      <c r="E325" s="12"/>
-      <c r="F325" s="12"/>
-    </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A326" s="11"/>
-      <c r="B326" s="12"/>
-      <c r="C326" s="12"/>
-      <c r="D326" s="12"/>
-      <c r="E326" s="12"/>
-      <c r="F326" s="12"/>
-    </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A327" s="11"/>
-      <c r="B327" s="12"/>
-      <c r="C327" s="12"/>
-      <c r="D327" s="12"/>
-      <c r="E327" s="12"/>
-      <c r="F327" s="12"/>
-    </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A328" s="11"/>
-      <c r="B328" s="12"/>
-      <c r="C328" s="12"/>
-      <c r="D328" s="12"/>
-      <c r="E328" s="12"/>
-      <c r="F328" s="12"/>
-    </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A329" s="11"/>
-      <c r="B329" s="12"/>
-      <c r="C329" s="12"/>
-      <c r="D329" s="12"/>
-      <c r="E329" s="12"/>
-      <c r="F329" s="12"/>
-    </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A330" s="11"/>
-      <c r="B330" s="12"/>
-      <c r="C330" s="12"/>
-      <c r="D330" s="12"/>
-      <c r="E330" s="12"/>
-      <c r="F330" s="12"/>
-    </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A331" s="11"/>
-      <c r="B331" s="12"/>
-      <c r="C331" s="12"/>
-      <c r="D331" s="12"/>
-      <c r="E331" s="12"/>
-      <c r="F331" s="12"/>
-    </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A332" s="11"/>
-      <c r="B332" s="12"/>
-      <c r="C332" s="12"/>
-      <c r="D332" s="12"/>
-      <c r="E332" s="12"/>
-      <c r="F332" s="12"/>
-    </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A333" s="11"/>
-      <c r="B333" s="12"/>
-      <c r="C333" s="12"/>
-      <c r="D333" s="12"/>
-      <c r="E333" s="12"/>
-      <c r="F333" s="12"/>
-    </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A334" s="11"/>
-      <c r="B334" s="12"/>
-      <c r="C334" s="12"/>
-      <c r="D334" s="12"/>
-      <c r="E334" s="12"/>
-      <c r="F334" s="12"/>
-    </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A335" s="11"/>
-      <c r="B335" s="12"/>
-      <c r="C335" s="12"/>
-      <c r="D335" s="12"/>
-      <c r="E335" s="12"/>
-      <c r="F335" s="12"/>
-    </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A336" s="11"/>
-      <c r="B336" s="12"/>
-      <c r="C336" s="12"/>
-      <c r="D336" s="12"/>
-      <c r="E336" s="12"/>
-      <c r="F336" s="12"/>
-    </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A337" s="11"/>
-      <c r="B337" s="12"/>
-      <c r="C337" s="12"/>
-      <c r="D337" s="12"/>
-      <c r="E337" s="12"/>
-      <c r="F337" s="12"/>
-    </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B337" s="72"/>
+      <c r="C337" s="72"/>
+      <c r="D337" s="72"/>
+      <c r="E337" s="72"/>
+      <c r="F337" s="72"/>
+      <c r="G337" s="73">
+        <f>G328-G336</f>
+        <v>86248</v>
+      </c>
+      <c r="H337" s="73"/>
+    </row>
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338" s="11"/>
       <c r="B338" s="12"/>
       <c r="C338" s="12"/>
@@ -8133,7 +8335,7 @@
       <c r="E338" s="12"/>
       <c r="F338" s="12"/>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339" s="11"/>
       <c r="B339" s="12"/>
       <c r="C339" s="12"/>
@@ -8141,7 +8343,7 @@
       <c r="E339" s="12"/>
       <c r="F339" s="12"/>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A340" s="11"/>
       <c r="B340" s="12"/>
       <c r="C340" s="12"/>
@@ -8149,7 +8351,7 @@
       <c r="E340" s="12"/>
       <c r="F340" s="12"/>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A341" s="11"/>
       <c r="B341" s="12"/>
       <c r="C341" s="12"/>
@@ -8157,191 +8359,303 @@
       <c r="E341" s="12"/>
       <c r="F341" s="12"/>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A342" s="9"/>
-      <c r="B342" s="76" t="s">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A342" s="11"/>
+      <c r="B342" s="12"/>
+      <c r="C342" s="12"/>
+      <c r="D342" s="12"/>
+      <c r="E342" s="12"/>
+      <c r="F342" s="12"/>
+    </row>
+    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A343" s="11"/>
+      <c r="B343" s="12"/>
+      <c r="C343" s="12"/>
+      <c r="D343" s="12"/>
+      <c r="E343" s="12"/>
+      <c r="F343" s="12"/>
+    </row>
+    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A344" s="11"/>
+      <c r="B344" s="12"/>
+      <c r="C344" s="12"/>
+      <c r="D344" s="12"/>
+      <c r="E344" s="12"/>
+      <c r="F344" s="12"/>
+    </row>
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A345" s="11"/>
+      <c r="B345" s="12"/>
+      <c r="C345" s="12"/>
+      <c r="D345" s="12"/>
+      <c r="E345" s="12"/>
+      <c r="F345" s="12"/>
+    </row>
+    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A346" s="11"/>
+      <c r="B346" s="12"/>
+      <c r="C346" s="12"/>
+      <c r="D346" s="12"/>
+      <c r="E346" s="12"/>
+      <c r="F346" s="12"/>
+    </row>
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A347" s="11"/>
+      <c r="B347" s="12"/>
+      <c r="C347" s="12"/>
+      <c r="D347" s="12"/>
+      <c r="E347" s="12"/>
+      <c r="F347" s="12"/>
+    </row>
+    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A348" s="11"/>
+      <c r="B348" s="12"/>
+      <c r="C348" s="12"/>
+      <c r="D348" s="12"/>
+      <c r="E348" s="12"/>
+      <c r="F348" s="12"/>
+    </row>
+    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A349" s="11"/>
+      <c r="B349" s="12"/>
+      <c r="C349" s="12"/>
+      <c r="D349" s="12"/>
+      <c r="E349" s="12"/>
+      <c r="F349" s="12"/>
+    </row>
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A350" s="11"/>
+      <c r="B350" s="12"/>
+      <c r="C350" s="12"/>
+      <c r="D350" s="12"/>
+      <c r="E350" s="12"/>
+      <c r="F350" s="12"/>
+    </row>
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A351" s="11"/>
+      <c r="B351" s="12"/>
+      <c r="C351" s="12"/>
+      <c r="D351" s="12"/>
+      <c r="E351" s="12"/>
+      <c r="F351" s="12"/>
+    </row>
+    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A352" s="11"/>
+      <c r="B352" s="12"/>
+      <c r="C352" s="12"/>
+      <c r="D352" s="12"/>
+      <c r="E352" s="12"/>
+      <c r="F352" s="12"/>
+    </row>
+    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A353" s="11"/>
+      <c r="B353" s="12"/>
+      <c r="C353" s="12"/>
+      <c r="D353" s="12"/>
+      <c r="E353" s="12"/>
+      <c r="F353" s="12"/>
+    </row>
+    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A354" s="11"/>
+      <c r="B354" s="12"/>
+      <c r="C354" s="12"/>
+      <c r="D354" s="12"/>
+      <c r="E354" s="12"/>
+      <c r="F354" s="12"/>
+    </row>
+    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A355" s="11"/>
+      <c r="B355" s="12"/>
+      <c r="C355" s="12"/>
+      <c r="D355" s="12"/>
+      <c r="E355" s="12"/>
+      <c r="F355" s="12"/>
+    </row>
+    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A356" s="9"/>
+      <c r="B356" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="C342" s="76"/>
-      <c r="D342" s="76"/>
-      <c r="E342" s="76"/>
-      <c r="F342" s="76"/>
-      <c r="G342" s="20"/>
-      <c r="H342" s="20"/>
-      <c r="I342" s="7">
-        <f>G311+H311</f>
-        <v>442.59</v>
-      </c>
-      <c r="J342" s="7">
-        <f>I342</f>
-        <v>442.59</v>
-      </c>
-    </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A343" s="5"/>
-      <c r="B343" s="77" t="s">
+      <c r="C356" s="84"/>
+      <c r="D356" s="84"/>
+      <c r="E356" s="84"/>
+      <c r="F356" s="84"/>
+      <c r="G356" s="20"/>
+      <c r="H356" s="20"/>
+      <c r="I356" s="7">
+        <f>G325+H325</f>
+        <v>475.09</v>
+      </c>
+      <c r="J356" s="7">
+        <f>I356</f>
+        <v>475.09</v>
+      </c>
+    </row>
+    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A357" s="5"/>
+      <c r="B357" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="C343" s="77"/>
-      <c r="D343" s="77"/>
-      <c r="E343" s="77"/>
-      <c r="F343" s="77"/>
-      <c r="I343" s="7">
+      <c r="C357" s="85"/>
+      <c r="D357" s="85"/>
+      <c r="E357" s="85"/>
+      <c r="F357" s="85"/>
+      <c r="I357" s="7">
         <v>300</v>
       </c>
-      <c r="J343" s="7">
+      <c r="J357" s="7">
         <v>200</v>
       </c>
     </row>
-    <row r="344" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A344" s="5"/>
-      <c r="B344" s="77" t="s">
+    <row r="358" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A358" s="5"/>
+      <c r="B358" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="C344" s="77"/>
-      <c r="D344" s="77"/>
-      <c r="E344" s="77"/>
-      <c r="F344" s="77"/>
-      <c r="I344" s="8">
-        <f>I343*I342</f>
-        <v>132777</v>
-      </c>
-      <c r="J344" s="8">
-        <f>J343*J342</f>
-        <v>88518</v>
-      </c>
-    </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A345" s="22"/>
-      <c r="B345" s="78" t="s">
+      <c r="C358" s="85"/>
+      <c r="D358" s="85"/>
+      <c r="E358" s="85"/>
+      <c r="F358" s="85"/>
+      <c r="I358" s="8">
+        <f>I357*I356</f>
+        <v>142527</v>
+      </c>
+      <c r="J358" s="8">
+        <f>J357*J356</f>
+        <v>95018</v>
+      </c>
+    </row>
+    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A359" s="22"/>
+      <c r="B359" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="C345" s="78"/>
-      <c r="D345" s="78"/>
-      <c r="E345" s="78"/>
-      <c r="F345" s="78"/>
-      <c r="G345" s="23"/>
-      <c r="H345" s="23"/>
-      <c r="I345" s="24"/>
-      <c r="J345" s="24"/>
-    </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A346" s="25">
+      <c r="C359" s="86"/>
+      <c r="D359" s="86"/>
+      <c r="E359" s="86"/>
+      <c r="F359" s="86"/>
+      <c r="G359" s="23"/>
+      <c r="H359" s="23"/>
+      <c r="I359" s="24"/>
+      <c r="J359" s="24"/>
+    </row>
+    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A360" s="25">
         <v>45109</v>
       </c>
-      <c r="B346" s="72" t="s">
+      <c r="B360" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="C346" s="72"/>
-      <c r="D346" s="72"/>
-      <c r="E346" s="72"/>
-      <c r="F346" s="72"/>
-      <c r="G346" s="26"/>
-      <c r="H346" s="26"/>
-      <c r="I346" s="27">
+      <c r="C360" s="81"/>
+      <c r="D360" s="81"/>
+      <c r="E360" s="81"/>
+      <c r="F360" s="81"/>
+      <c r="G360" s="26"/>
+      <c r="H360" s="26"/>
+      <c r="I360" s="27">
         <v>10000</v>
       </c>
-      <c r="J346" s="27">
+      <c r="J360" s="27">
         <v>10000</v>
       </c>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A347" s="25"/>
-      <c r="B347" s="28"/>
-      <c r="C347" s="28"/>
-      <c r="D347" s="28"/>
-      <c r="E347" s="28"/>
-      <c r="F347" s="28"/>
-      <c r="G347" s="26"/>
-      <c r="H347" s="26"/>
-      <c r="I347" s="29"/>
-      <c r="J347" s="29"/>
-    </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A348" s="25"/>
-      <c r="B348" s="28"/>
-      <c r="C348" s="28"/>
-      <c r="D348" s="28"/>
-      <c r="E348" s="28"/>
-      <c r="F348" s="28"/>
-      <c r="G348" s="26"/>
-      <c r="H348" s="26"/>
-      <c r="I348" s="29"/>
-      <c r="J348" s="29"/>
-    </row>
-    <row r="349" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A349" s="25"/>
-      <c r="B349" s="73" t="s">
+    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A361" s="25"/>
+      <c r="B361" s="28"/>
+      <c r="C361" s="28"/>
+      <c r="D361" s="28"/>
+      <c r="E361" s="28"/>
+      <c r="F361" s="28"/>
+      <c r="G361" s="26"/>
+      <c r="H361" s="26"/>
+      <c r="I361" s="29"/>
+      <c r="J361" s="29"/>
+    </row>
+    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A362" s="25"/>
+      <c r="B362" s="28"/>
+      <c r="C362" s="28"/>
+      <c r="D362" s="28"/>
+      <c r="E362" s="28"/>
+      <c r="F362" s="28"/>
+      <c r="G362" s="26"/>
+      <c r="H362" s="26"/>
+      <c r="I362" s="29"/>
+      <c r="J362" s="29"/>
+    </row>
+    <row r="363" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A363" s="25"/>
+      <c r="B363" s="82" t="s">
         <v>62</v>
       </c>
-      <c r="C349" s="73"/>
-      <c r="D349" s="73"/>
-      <c r="E349" s="73"/>
-      <c r="F349" s="73"/>
-      <c r="G349" s="26"/>
-      <c r="H349" s="26"/>
-      <c r="I349" s="30">
-        <f>SUM(I346:I348)</f>
+      <c r="C363" s="82"/>
+      <c r="D363" s="82"/>
+      <c r="E363" s="82"/>
+      <c r="F363" s="82"/>
+      <c r="G363" s="26"/>
+      <c r="H363" s="26"/>
+      <c r="I363" s="30">
+        <f>SUM(I360:I362)</f>
         <v>10000</v>
       </c>
-      <c r="J349" s="30">
-        <f>SUM(J346:J348)</f>
+      <c r="J363" s="30">
+        <f>SUM(J360:J362)</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="350" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A350" s="31">
+    <row r="364" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A364" s="31">
         <v>45109</v>
       </c>
-      <c r="B350" s="71" t="s">
+      <c r="B364" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="C350" s="71"/>
-      <c r="D350" s="71"/>
-      <c r="E350" s="71"/>
-      <c r="F350" s="71"/>
-      <c r="G350" s="32"/>
-      <c r="H350" s="32"/>
-      <c r="I350" s="33">
-        <f>I344-I349</f>
-        <v>122777</v>
-      </c>
-      <c r="J350" s="33">
-        <f>J344-J349</f>
-        <v>78518</v>
+      <c r="C364" s="80"/>
+      <c r="D364" s="80"/>
+      <c r="E364" s="80"/>
+      <c r="F364" s="80"/>
+      <c r="G364" s="32"/>
+      <c r="H364" s="32"/>
+      <c r="I364" s="33">
+        <f>I358-I363</f>
+        <v>132527</v>
+      </c>
+      <c r="J364" s="33">
+        <f>J358-J363</f>
+        <v>85018</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="G314:H314"/>
-    <mergeCell ref="A323:F323"/>
-    <mergeCell ref="G323:H323"/>
-    <mergeCell ref="B315:F315"/>
-    <mergeCell ref="B316:F316"/>
-    <mergeCell ref="B322:F322"/>
-    <mergeCell ref="G316:H316"/>
-    <mergeCell ref="G317:H317"/>
-    <mergeCell ref="G322:H322"/>
-    <mergeCell ref="G319:H319"/>
-    <mergeCell ref="G320:H320"/>
-    <mergeCell ref="G321:H321"/>
-    <mergeCell ref="G318:H318"/>
-    <mergeCell ref="B318:F318"/>
-    <mergeCell ref="B317:F317"/>
-    <mergeCell ref="B319:F319"/>
-    <mergeCell ref="B350:F350"/>
-    <mergeCell ref="B346:F346"/>
-    <mergeCell ref="B349:F349"/>
-    <mergeCell ref="A312:F312"/>
-    <mergeCell ref="A311:F311"/>
-    <mergeCell ref="A313:F313"/>
-    <mergeCell ref="A314:F314"/>
-    <mergeCell ref="B320:F320"/>
-    <mergeCell ref="B321:F321"/>
-    <mergeCell ref="B342:F342"/>
-    <mergeCell ref="B343:F343"/>
-    <mergeCell ref="B344:F344"/>
-    <mergeCell ref="B345:F345"/>
+    <mergeCell ref="B364:F364"/>
+    <mergeCell ref="B360:F360"/>
+    <mergeCell ref="B363:F363"/>
+    <mergeCell ref="A326:F326"/>
+    <mergeCell ref="A325:F325"/>
+    <mergeCell ref="A327:F327"/>
+    <mergeCell ref="A328:F328"/>
+    <mergeCell ref="B334:F334"/>
+    <mergeCell ref="B335:F335"/>
+    <mergeCell ref="B356:F356"/>
+    <mergeCell ref="B357:F357"/>
+    <mergeCell ref="B358:F358"/>
+    <mergeCell ref="B359:F359"/>
+    <mergeCell ref="G328:H328"/>
+    <mergeCell ref="A337:F337"/>
+    <mergeCell ref="G337:H337"/>
+    <mergeCell ref="B329:F329"/>
+    <mergeCell ref="B330:F330"/>
+    <mergeCell ref="B336:F336"/>
+    <mergeCell ref="G330:H330"/>
+    <mergeCell ref="G331:H331"/>
+    <mergeCell ref="G336:H336"/>
+    <mergeCell ref="G333:H333"/>
+    <mergeCell ref="G334:H334"/>
+    <mergeCell ref="G335:H335"/>
+    <mergeCell ref="G332:H332"/>
+    <mergeCell ref="B332:F332"/>
+    <mergeCell ref="B331:F331"/>
+    <mergeCell ref="B333:F333"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -8353,7 +8667,7 @@
   <dimension ref="A1:D117"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9157,10 +9471,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6078F90-1BFA-44D9-9906-5A72B5F0645C}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9502,161 +9816,322 @@
         <v>2550</v>
       </c>
     </row>
-    <row r="39" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="51"/>
-      <c r="B39" s="52"/>
-      <c r="C39" s="53"/>
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="48"/>
+      <c r="B39" s="66" t="s">
+        <v>311</v>
+      </c>
+      <c r="C39" s="89">
+        <v>4800</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="43"/>
-      <c r="B40" s="43" t="s">
-        <v>247</v>
-      </c>
-      <c r="C40" s="46">
-        <f>SUM(C2:C39)</f>
-        <v>20600</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="55">
-        <v>45690</v>
-      </c>
-      <c r="B42" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" s="54">
-        <v>2300</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="55"/>
-      <c r="B43" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="C43" s="54">
-        <v>2250</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="55">
-        <v>45804</v>
-      </c>
-      <c r="B44" s="48" t="s">
-        <v>278</v>
-      </c>
-      <c r="C44" s="54">
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="55">
-        <v>45839</v>
-      </c>
-      <c r="B45" s="48" t="s">
-        <v>278</v>
-      </c>
-      <c r="C45" s="54">
-        <v>4200</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="55"/>
-      <c r="B46" s="48"/>
-      <c r="C46" s="54">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="55">
-        <v>46266</v>
-      </c>
-      <c r="B47" s="48"/>
-      <c r="C47" s="54">
-        <v>2100</v>
-      </c>
+      <c r="A40" s="48"/>
+      <c r="B40" s="67" t="s">
+        <v>312</v>
+      </c>
+      <c r="C40" s="90"/>
+    </row>
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="48"/>
+      <c r="B41" s="67" t="s">
+        <v>313</v>
+      </c>
+      <c r="C41" s="90"/>
+    </row>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="48"/>
+      <c r="B42" s="67" t="s">
+        <v>314</v>
+      </c>
+      <c r="C42" s="90"/>
+    </row>
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="48"/>
+      <c r="B43" s="67" t="s">
+        <v>316</v>
+      </c>
+      <c r="C43" s="90"/>
+    </row>
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="48"/>
+      <c r="B44" s="67" t="s">
+        <v>315</v>
+      </c>
+      <c r="C44" s="90"/>
+    </row>
+    <row r="45" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="48"/>
+      <c r="B45" s="68" t="s">
+        <v>317</v>
+      </c>
+      <c r="C45" s="91"/>
+    </row>
+    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="48"/>
+      <c r="B46" s="66" t="s">
+        <v>329</v>
+      </c>
+      <c r="C46" s="87">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="48"/>
+      <c r="B47" s="67" t="s">
+        <v>319</v>
+      </c>
+      <c r="C47" s="92"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="48"/>
-      <c r="B48" s="48"/>
-      <c r="C48" s="54"/>
+      <c r="B48" s="67" t="s">
+        <v>321</v>
+      </c>
+      <c r="C48" s="92"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="43"/>
-      <c r="B49" s="43" t="s">
+      <c r="A49" s="48"/>
+      <c r="B49" s="67" t="s">
+        <v>318</v>
+      </c>
+      <c r="C49" s="92"/>
+    </row>
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="48"/>
+      <c r="B50" s="67" t="s">
+        <v>320</v>
+      </c>
+      <c r="C50" s="92"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="48"/>
+      <c r="B51" s="67" t="s">
+        <v>322</v>
+      </c>
+      <c r="C51" s="92"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="48"/>
+      <c r="B52" s="67" t="s">
+        <v>323</v>
+      </c>
+      <c r="C52" s="92"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="48"/>
+      <c r="B53" s="67" t="s">
+        <v>324</v>
+      </c>
+      <c r="C53" s="92"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="48"/>
+      <c r="B54" s="67" t="s">
+        <v>325</v>
+      </c>
+      <c r="C54" s="92"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="48"/>
+      <c r="B55" s="67" t="s">
+        <v>326</v>
+      </c>
+      <c r="C55" s="92"/>
+    </row>
+    <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="48"/>
+      <c r="B56" s="67" t="s">
+        <v>327</v>
+      </c>
+      <c r="C56" s="92"/>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="48"/>
+      <c r="B57" s="68" t="s">
+        <v>328</v>
+      </c>
+      <c r="C57" s="88"/>
+    </row>
+    <row r="58" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="51"/>
+      <c r="B58" s="52"/>
+      <c r="C58" s="53"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="43"/>
+      <c r="B59" s="43" t="s">
+        <v>247</v>
+      </c>
+      <c r="C59" s="46">
+        <f>SUM(C2:C58)</f>
+        <v>32900</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="55">
+        <v>45690</v>
+      </c>
+      <c r="B61" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="C61" s="54">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="55"/>
+      <c r="B62" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="C62" s="54">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="55">
+        <v>45804</v>
+      </c>
+      <c r="B63" s="48" t="s">
+        <v>278</v>
+      </c>
+      <c r="C63" s="54">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="55">
+        <v>45839</v>
+      </c>
+      <c r="B64" s="48" t="s">
+        <v>278</v>
+      </c>
+      <c r="C64" s="54">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="55"/>
+      <c r="B65" s="48"/>
+      <c r="C65" s="54">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="55">
+        <v>46266</v>
+      </c>
+      <c r="B66" s="48" t="s">
+        <v>249</v>
+      </c>
+      <c r="C66" s="54">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="55"/>
+      <c r="B67" s="48" t="s">
+        <v>249</v>
+      </c>
+      <c r="C67" s="54">
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="55">
+        <v>46073</v>
+      </c>
+      <c r="B68" s="48" t="s">
+        <v>249</v>
+      </c>
+      <c r="C68" s="54">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="55"/>
+      <c r="B69" s="48"/>
+      <c r="C69" s="54"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="48"/>
+      <c r="B70" s="48"/>
+      <c r="C70" s="54"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="43"/>
+      <c r="B71" s="43" t="s">
         <v>252</v>
       </c>
-      <c r="C49" s="46">
-        <f>SUM(C41:C48)</f>
-        <v>18050</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6" t="s">
+      <c r="C71" s="46">
+        <f>SUM(C60:C70)</f>
+        <v>25400</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="6"/>
+      <c r="B72" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="C50" s="47">
-        <f>C40-C49</f>
-        <v>2550</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="13" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="13" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="13" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B55" s="13" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="13" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="13" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="13" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="13" t="s">
-        <v>309</v>
+      <c r="C72" s="47">
+        <f>C59-C71</f>
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B76" s="13" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B77" s="13" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B78" s="13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B79" s="13" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B80" s="13" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B81" s="13" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B82" s="13" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="C46:C57"/>
+    <mergeCell ref="C39:C45"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="C15:C19"/>
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="C32:C34"/>
     <mergeCell ref="C28:C31"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="C22:C27"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="C15:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>